<commit_message>
removed quotes and upgraded to EMLassemblyline 2.12.1
</commit_message>
<xml_diff>
--- a/IFCB-EN608-metadata.xlsx
+++ b/IFCB-EN608-metadata.xlsx
@@ -197,9 +197,6 @@
     <t>Bacillariophyceae</t>
   </si>
   <si>
-    <t>other than diatoms, dinoflagellates, or haptophytes</t>
-  </si>
-  <si>
     <t>Haptophyta</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>concentration likely valid for this taxon when IFCB triggering only on chlorophyll fluorescence</t>
+  </si>
+  <si>
+    <t>other than diatoms dinoflagellates or haptophytes</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -612,7 +614,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -623,7 +625,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -631,10 +633,10 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -642,32 +644,32 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -855,22 +857,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>69</v>
-      </c>
-      <c r="F7" t="s">
-        <v>70</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -1023,36 +1025,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
       </c>
       <c r="D2">
         <v>1.0000000000000001E-18</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D3">
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
categorical variables not quite working yet for EML
</commit_message>
<xml_diff>
--- a/IFCB-EN608-metadata.xlsx
+++ b/IFCB-EN608-metadata.xlsx
@@ -12,10 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
-    <sheet name="CategoricalVariables" sheetId="5" r:id="rId1"/>
-    <sheet name="Personnel" sheetId="2" r:id="rId2"/>
-    <sheet name="Keywords" sheetId="3" r:id="rId3"/>
-    <sheet name="CustomUnits" sheetId="4" r:id="rId4"/>
+    <sheet name="Personnel" sheetId="2" r:id="rId1"/>
+    <sheet name="Keywords" sheetId="3" r:id="rId2"/>
+    <sheet name="CustomUnits" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>keyword</t>
   </si>
@@ -125,18 +124,6 @@
     <t>metadataProvider</t>
   </si>
   <si>
-    <t>attribute</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>higherClassification_group</t>
-  </si>
-  <si>
     <t>Emily</t>
   </si>
   <si>
@@ -191,27 +178,6 @@
     <t>populations</t>
   </si>
   <si>
-    <t>Dinoflagellata</t>
-  </si>
-  <si>
-    <t>Bacillariophyceae</t>
-  </si>
-  <si>
-    <t>Haptophyta</t>
-  </si>
-  <si>
-    <t>urn:lsid:marinespecies.org:taxname:148899</t>
-  </si>
-  <si>
-    <t>urn:lsid:marinespecies.org:taxname:146203</t>
-  </si>
-  <si>
-    <t>urn:lsid:marinespecies.org:taxname:369190</t>
-  </si>
-  <si>
-    <t>taxon that can not be classified under any of the 3 listed higher level phytoplankton groups</t>
-  </si>
-  <si>
     <t>cubicMicrometers</t>
   </si>
   <si>
@@ -249,9 +215,6 @@
   </si>
   <si>
     <t>area</t>
-  </si>
-  <si>
-    <t>other than diatoms dinoflagellates or haptophytes</t>
   </si>
 </sst>
 </file>
@@ -573,84 +536,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" customWidth="1"/>
-    <col min="3" max="3" width="32.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -725,16 +613,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>27</v>
@@ -751,16 +639,16 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
@@ -800,16 +688,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -826,22 +714,22 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
         <v>31</v>
@@ -861,7 +749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -884,7 +772,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -892,7 +780,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -900,7 +788,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -908,7 +796,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -916,7 +804,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -924,7 +812,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -932,7 +820,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -940,7 +828,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -948,7 +836,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -962,7 +850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -994,36 +882,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>1.0000000000000001E-18</v>
       </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D3">
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
accounts for 7 ROIs with features NA
</commit_message>
<xml_diff>
--- a/IFCB-EN608-metadata.xlsx
+++ b/IFCB-EN608-metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>keyword</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>area</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Open Biological and Biomedical Ontology (OBO)</t>
   </si>
 </sst>
 </file>
@@ -538,7 +544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -753,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +849,12 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated concentrationFlag, personnel, and methods
</commit_message>
<xml_diff>
--- a/IFCB-EN608-metadata.xlsx
+++ b/IFCB-EN608-metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>keyword</t>
   </si>
@@ -221,6 +221,30 @@
   </si>
   <si>
     <t>Open Biological and Biomedical Ontology (OBO)</t>
+  </si>
+  <si>
+    <t>E. Taylor</t>
+  </si>
+  <si>
+    <t>Crockford</t>
+  </si>
+  <si>
+    <t>ecrockford@whoi.edu</t>
+  </si>
+  <si>
+    <t>technician</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Futrelle</t>
+  </si>
+  <si>
+    <t>jfutrelle@whoi.edu</t>
+  </si>
+  <si>
+    <t>softwareDeveloper</t>
   </si>
 </sst>
 </file>
@@ -542,9 +566,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -694,19 +718,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
@@ -720,25 +744,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
@@ -747,6 +765,64 @@
         <v>25</v>
       </c>
       <c r="J7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -759,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated title, methods, missing value code for features
</commit_message>
<xml_diff>
--- a/IFCB-EN608-metadata.xlsx
+++ b/IFCB-EN608-metadata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="74">
   <si>
     <t>keyword</t>
   </si>
@@ -220,9 +220,6 @@
     <t>image</t>
   </si>
   <si>
-    <t>Open Biological and Biomedical Ontology (OBO)</t>
-  </si>
-  <si>
     <t>E. Taylor</t>
   </si>
   <si>
@@ -245,6 +242,12 @@
   </si>
   <si>
     <t>softwareDeveloper</t>
+  </si>
+  <si>
+    <t>0000-0002-6839-2579</t>
+  </si>
+  <si>
+    <t>OBO Open Biological and Biomedical Ontology</t>
   </si>
 </sst>
 </file>
@@ -568,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,6 +683,9 @@
       <c r="E4" t="s">
         <v>47</v>
       </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
       <c r="G4" t="s">
         <v>27</v>
       </c>
@@ -718,19 +724,19 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
         <v>65</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>66</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
@@ -744,19 +750,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>71</v>
-      </c>
-      <c r="G7" t="s">
-        <v>72</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
@@ -835,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -929,7 +935,7 @@
         <v>63</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>